<commit_message>
Update PLANILLA DE EVALUACIÓN AVANCE FASE 2.xlsx
</commit_message>
<xml_diff>
--- a/Fase 2/Evidencias Grupales/PLANILLA DE EVALUACIÓN AVANCE FASE 2.xlsx
+++ b/Fase 2/Evidencias Grupales/PLANILLA DE EVALUACIÓN AVANCE FASE 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://duoccl0-my.sharepoint.com/personal/ge_galan_profesor_duoc_cl/Documents/2024-2/Clases/CAPSTONE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afran\OneDrive\Documentos\GitHub\capstone2024\Fase 2\Evidencias Grupales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="628" documentId="8_{2EFDF332-31E9-4C74-A6B5-E695634C1C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{963FD2AD-F390-4590-BC90-915A09DBAA60}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AACC01B-5486-4742-B14C-48FB77D00DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVALUACION2" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>PUNTOS</t>
   </si>
@@ -276,6 +276,15 @@
   </si>
   <si>
     <t>No generan evidencias dentro del repositorio  del proyecto del aporte de cada uno de los integrantes del equipo por lo que no se permite identificar la equidad en el trabajo y la participación de cada estudiante</t>
+  </si>
+  <si>
+    <t>Nicolas Moreno Alegria</t>
+  </si>
+  <si>
+    <t>Benjamin Tagle</t>
+  </si>
+  <si>
+    <t>Alejandro Escobedo Miño</t>
   </si>
 </sst>
 </file>
@@ -762,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -860,6 +869,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="9" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -883,9 +901,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -895,31 +910,19 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1251,10 +1254,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K895"/>
+  <dimension ref="A1:N895"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -1271,12 +1274,15 @@
     <col min="12" max="24" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="25"/>
+    </row>
+    <row r="2" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1284,83 +1290,89 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
       <c r="C4" s="5">
         <f>EVALUACION2!$C$22</f>
         <v>7</v>
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="25"/>
+      <c r="B5" s="25" t="s">
+        <v>64</v>
+      </c>
       <c r="C5" s="5">
         <f>EVALUACION2!$C$22</f>
         <v>7</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="25" t="s">
+        <v>65</v>
+      </c>
       <c r="C6" s="5">
         <f>EVALUACION2!$C$22</f>
         <v>7</v>
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="18" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37" t="s">
+    <row r="11" spans="1:14" ht="18" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="14"/>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="43"/>
-    </row>
-    <row r="12" spans="1:11" ht="14.4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="46"/>
+    </row>
+    <row r="12" spans="1:14" ht="14.4" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="41"/>
       <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="42" t="s">
+      <c r="C12" s="43"/>
+      <c r="D12" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="42" t="s">
+      <c r="E12" s="46"/>
+      <c r="F12" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="43"/>
-      <c r="H12" s="45" t="s">
+      <c r="G12" s="46"/>
+      <c r="H12" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="42" t="s">
+      <c r="I12" s="46"/>
+      <c r="J12" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="43"/>
-    </row>
-    <row r="13" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
+      <c r="K12" s="46"/>
+    </row>
+    <row r="13" spans="1:14" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="42"/>
       <c r="B13" s="28" t="str">
         <f>RUBRICA!A4</f>
         <v xml:space="preserve">1. Propone ajustes al Proyecto APT considerando dificultades, facilitadores y retroalimentación. </v>
@@ -1401,8 +1413,8 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="26.4" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
+    <row r="14" spans="1:14" ht="26.4" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="42"/>
       <c r="B14" s="28" t="str">
         <f>RUBRICA!A5</f>
         <v>2. Aplica una metodología que permite el logro de los objetivos propuestos, de acuerdo a los estándares de la disciplina.</v>
@@ -1443,8 +1455,8 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="36" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
+    <row r="15" spans="1:14" ht="36" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="42"/>
       <c r="B15" s="28" t="str">
         <f>RUBRICA!A6</f>
         <v>3. Genera evidencias que dan cuenta del avance del Proyecto APT en relación a documentación, programación y almacenamiento de datos , de acuerdo a lo planificado por el equipo y que cumpla con estándares de desarrollo de la industria</v>
@@ -1485,8 +1497,8 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
+    <row r="16" spans="1:14" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="42"/>
       <c r="B16" s="28" t="str">
         <f>RUBRICA!A7</f>
         <v>4. Utiliza de manera precisa el lenguaje técnico en los entregables de acuerdo con lo requerido por la disciplina.</v>
@@ -1528,7 +1540,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="39"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="28" t="str">
         <f>RUBRICA!A8</f>
         <v xml:space="preserve">5. Utiliza reglas de redacción, ortografía (literal, puntual, acentual) y las normas para citas y referencias. </v>
@@ -1570,7 +1582,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="24" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="28" t="str">
         <f>RUBRICA!A9</f>
         <v>6. Entrega la documentación y evidencias requerida por la asignatura de acuerdo a la estrucutra y nombres solicitados, guardando todas las evidencias de avances en Git</v>
@@ -1612,7 +1624,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="36" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="28" t="str">
         <f>RUBRICA!A10</f>
         <v>7.- Generan evidencias claras dentro del repositorio  del aporte de cada uno de los integrantes del equipo que permitan identificar la equidad en el trabajo y la participación de cada estudiante.</v>
@@ -1654,7 +1666,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="36" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
+      <c r="A20" s="42"/>
       <c r="B20" s="28" t="str">
         <f>RUBRICA!A11</f>
         <v>8. Demuestra un trabajo en equipo en donde todos los miembros del equipo expresan con fluidez el conocimiento del tema expuesto y  participan de las actividades planificadas en el proyecto</v>
@@ -1696,7 +1708,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="38"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="27" t="s">
         <v>4</v>
       </c>
@@ -1726,7 +1738,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="40"/>
+      <c r="A22" s="43"/>
       <c r="B22" s="30" t="s">
         <v>13</v>
       </c>
@@ -2664,7 +2676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B396D1B-8A63-4A90-BA20-D34AC13A3962}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2674,25 +2686,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="46" t="s">
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="49" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="52" t="s">
+      <c r="A2" s="50"/>
+      <c r="B2" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="55" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="21" t="s">
@@ -2701,22 +2713,22 @@
       <c r="E2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="47"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56">
+      <c r="A3" s="50"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="37">
         <v>-0.3</v>
       </c>
-      <c r="E3" s="56">
+      <c r="E3" s="37">
         <v>0</v>
       </c>
-      <c r="F3" s="48"/>
+      <c r="F3" s="54"/>
     </row>
     <row r="4" spans="1:6" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="24" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="24" t="s">
@@ -2736,7 +2748,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="24" t="s">
@@ -2756,7 +2768,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="24" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="24" t="s">
@@ -2776,7 +2788,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="24" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="24" t="s">
@@ -2796,7 +2808,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="24" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="24" t="s">
@@ -2811,12 +2823,12 @@
       <c r="E8" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="57">
+      <c r="F8" s="38">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="24" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="24" t="s">
@@ -2836,19 +2848,19 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="58" t="s">
+      <c r="D10" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="39" t="s">
         <v>62</v>
       </c>
       <c r="F10" s="32">
@@ -2856,7 +2868,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="24" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="24" t="s">
@@ -8116,7 +8128,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
@@ -8127,7 +8139,7 @@
       <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="54"/>
+      <c r="A2" s="58"/>
       <c r="B2" s="9" t="s">
         <v>5</v>
       </c>

</xml_diff>